<commit_message>
[DN] Bundle Of Traits - 2600986277 업데이트
</commit_message>
<xml_diff>
--- a/Data/[DN] Bundle Of Traits - 2600986277/2600986277.xlsx
+++ b/Data/[DN] Bundle Of Traits - 2600986277/2600986277.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stone\Desktop\새 폴더 (2)\RimworldExtractor 0.8.6\[DN] Bundle Of Traits - 2600986277\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\[DN] Bundle Of Traits - 2600986277\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B42F616-7469-4D8A-8607-9211A379C208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39639E7E-4702-49CF-84FB-85B76583F277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240523" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="1458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2529" uniqueCount="1472">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -4412,6 +4412,62 @@
   </si>
   <si>
     <t>더미</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>폐소공포증</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>통각과민</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(은)는 통증에 극도로 민감하게 반응하는 희귀 질환을 앓고 있으며, 실제 입은 상처보다 훨씬 강한 통증을 느낍니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>기면증에서 깨어남</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>내가… 잠에 들었었나?</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>기면증</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN_nameDef}(이)가 기면증으로 인해 잠들었습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태: 기면증</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{PAWN}의 기면증이 종료되었습니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>fleeing</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>도피</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>도피 헤디프</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>신진대사</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>신진대사 헤디프</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4831,8 +4887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F356"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="C339" workbookViewId="0">
+      <selection activeCell="F343" sqref="F343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -5897,10 +5953,10 @@
         <v>192</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>193</v>
+        <v>1467</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>1456</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
@@ -5917,7 +5973,7 @@
         <v>193</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>1456</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
@@ -5934,7 +5990,7 @@
         <v>198</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>1456</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
@@ -5951,7 +6007,7 @@
         <v>201</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1456</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
@@ -5968,7 +6024,7 @@
         <v>201</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>1456</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
@@ -5985,7 +6041,7 @@
         <v>206</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>1456</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
@@ -6733,7 +6789,7 @@
         <v>339</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>1456</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.45">
@@ -6750,7 +6806,7 @@
         <v>342</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>1456</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.45">
@@ -6767,7 +6823,7 @@
         <v>345</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>1456</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.45">
@@ -6784,7 +6840,7 @@
         <v>348</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>1456</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.45">
@@ -9147,7 +9203,7 @@
         <v>746</v>
       </c>
       <c r="F253" s="1" t="s">
-        <v>1456</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.45">
@@ -9164,7 +9220,7 @@
         <v>749</v>
       </c>
       <c r="F254" s="1" t="s">
-        <v>1456</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.45">
@@ -10609,7 +10665,7 @@
         <v>1003</v>
       </c>
       <c r="F339" s="1" t="s">
-        <v>1071</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="340" spans="1:6" x14ac:dyDescent="0.45">
@@ -10711,7 +10767,7 @@
         <v>1021</v>
       </c>
       <c r="F345" s="1" t="s">
-        <v>1456</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="346" spans="1:6" x14ac:dyDescent="0.45">
@@ -10728,7 +10784,7 @@
         <v>1024</v>
       </c>
       <c r="F346" s="1" t="s">
-        <v>1456</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="347" spans="1:6" x14ac:dyDescent="0.45">

</xml_diff>